<commit_message>
template and custom functions update
</commit_message>
<xml_diff>
--- a/2_CodeMappingTemplates/Regulatory/XXre_Regulatory Schema Mapping to WaDE.xlsx
+++ b/2_CodeMappingTemplates/Regulatory/XXre_Regulatory Schema Mapping to WaDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\2_CodeMappingTemplates\Regulatory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF890CEE-566F-48B1-AFA4-33954CE3978A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8578719-6132-439D-BCDB-413788B86F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12456" tabRatio="645" activeTab="2" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="28680" yWindow="-1380" windowWidth="38640" windowHeight="21120" tabRatio="645" activeTab="2" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -1734,7 +1734,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>